<commit_message>
Updated the template for example data. Renamed to Tag
</commit_message>
<xml_diff>
--- a/DB/Vorlagen für BSP-Daten/Event.xlsx
+++ b/DB/Vorlagen für BSP-Daten/Event.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Henri\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Henri\Documents\GitHub\location-based-recommendations\DB\Vorlagen für BSP-Daten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{127E2290-725A-47A8-A4EF-90D3ABF553E0}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5E0E1A8-233A-498E-8985-CC7738454964}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="450" windowWidth="11490" windowHeight="4590" xr2:uid="{9534E945-7C34-4513-B816-820DF00FA453}"/>
+    <workbookView xWindow="0" yWindow="900" windowWidth="11490" windowHeight="4590" xr2:uid="{9534E945-7C34-4513-B816-820DF00FA453}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>event_id</t>
   </si>
@@ -37,6 +37,9 @@
   </si>
   <si>
     <t>venue_id</t>
+  </si>
+  <si>
+    <t>time</t>
   </si>
 </sst>
 </file>
@@ -388,10 +391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0347189E-8D83-4E0C-A6D6-6CE70796E6AA}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -400,7 +403,7 @@
     <col min="3" max="3" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -411,6 +414,9 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>